<commit_message>
Python mini project day 5
</commit_message>
<xml_diff>
--- a/VM IP's.xlsx
+++ b/VM IP's.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\OneDrive\Desktop\MMC\mmc_training_0725\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FF67AB5-F385-4D15-9ACD-BAB7558591AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E450F717-F265-4CCC-8EDA-C673BCEFD46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{CB76107F-2CB8-4EA2-9095-03A349661015}"/>
+    <workbookView xWindow="0" yWindow="1869" windowWidth="21651" windowHeight="11125" activeTab="2" xr2:uid="{CB76107F-2CB8-4EA2-9095-03A349661015}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +90,39 @@
   </si>
   <si>
     <t>Devaanshi Chaturvedi</t>
+  </si>
+  <si>
+    <t>user-one</t>
+  </si>
+  <si>
+    <t>user-two</t>
+  </si>
+  <si>
+    <t>user-three</t>
+  </si>
+  <si>
+    <t>user-four</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>user-five</t>
+  </si>
+  <si>
+    <t>user-six</t>
+  </si>
+  <si>
+    <t>user-seven</t>
   </si>
 </sst>
 </file>
@@ -149,13 +184,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2615B7-86F6-4AEC-BC45-8397EC0FC64B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -482,7 +518,7 @@
     <col min="2" max="2" width="31.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,47 +526,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -538,20 +595,252 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.15" x14ac:dyDescent="0.7">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDEDA9C-F605-456B-89DC-D6ECA1C34EFA}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B9" sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="34.299999999999997" customHeight="1" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="36.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.921875" customWidth="1"/>
+    <col min="3" max="3" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0860176F-892F-432D-BC4F-CE1F33E0B01D}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.85" customHeight="1" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="35.765625" customWidth="1"/>
+    <col min="2" max="2" width="35.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="25.85" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 5, 6 and 7
</commit_message>
<xml_diff>
--- a/VM IP's.xlsx
+++ b/VM IP's.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\OneDrive\Desktop\MMC\mmc_training_0725\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D52721-6E00-47FE-80B5-C7A1DCD7E157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5569956E-05D6-4619-83F3-2F25D1EA092A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1869" windowWidth="21651" windowHeight="11125" activeTab="2" xr2:uid="{CB76107F-2CB8-4EA2-9095-03A349661015}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{CB76107F-2CB8-4EA2-9095-03A349661015}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -741,7 +741,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.85" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>